<commit_message>
commit as of 04/01/2020 -Entity in user service
</commit_message>
<xml_diff>
--- a/doc/PusherDetails.xlsx
+++ b/doc/PusherDetails.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623AC67E-04E1-4793-8099-8A82816202C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Sr No.</t>
   </si>
@@ -134,12 +135,24 @@
   <si>
     <t>UpdateStatus(NOTPRESENT,SEATED,INCOMPLETE)</t>
   </si>
+  <si>
+    <t>RESET_ORGANIZATION_PUSHER</t>
+  </si>
+  <si>
+    <t>ADD</t>
+  </si>
+  <si>
+    <t>UPDATE</t>
+  </si>
+  <si>
+    <t>DELETE/INCOMPLETE/NOTPRESENT/SEATED</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,7 +189,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -199,11 +212,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -218,12 +251,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -270,7 +314,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -302,9 +346,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -336,6 +398,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -511,22 +591,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
     <col min="2" max="2" width="32.7109375" customWidth="1"/>
     <col min="3" max="3" width="33.140625" customWidth="1"/>
     <col min="4" max="4" width="39.7109375" customWidth="1"/>
+    <col min="5" max="5" width="44.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -539,8 +620,11 @@
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E2" s="8" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="45">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -554,7 +638,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="165">
+    <row r="4" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -568,7 +652,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="60">
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -581,8 +665,11 @@
       <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="E5" s="9" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" ht="315">
+    <row r="6" spans="1:5" ht="315" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -595,8 +682,11 @@
       <c r="D6" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="E6" s="9" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" ht="285">
+    <row r="7" spans="1:5" ht="285" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -609,8 +699,11 @@
       <c r="D7" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="E7" s="10" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" ht="195">
+    <row r="8" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -623,8 +716,11 @@
       <c r="D8" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="E8" s="10" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9" s="1"/>
     </row>
   </sheetData>
@@ -634,24 +730,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
commit as of 01/04/2020 Entity mapping issue solved
</commit_message>
<xml_diff>
--- a/doc/PusherDetails.xlsx
+++ b/doc/PusherDetails.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623AC67E-04E1-4793-8099-8A82816202C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA1375C-3A86-44E7-954E-0D93740BEC09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>Sr No.</t>
   </si>
@@ -146,6 +146,27 @@
   </si>
   <si>
     <t>DELETE/INCOMPLETE/NOTPRESENT/SEATED</t>
+  </si>
+  <si>
+    <t>ADD_LANGUAGE_PUSHER</t>
+  </si>
+  <si>
+    <t>Add language</t>
+  </si>
+  <si>
+    <t>delete language</t>
+  </si>
+  <si>
+    <t>Update Organization setting</t>
+  </si>
+  <si>
+    <t>ORG_SETTING_PUSHER</t>
+  </si>
+  <si>
+    <t>REFRESH_LANGUAGE_PUSHER</t>
+  </si>
+  <si>
+    <t>NOTIFY_USER</t>
   </si>
 </sst>
 </file>
@@ -189,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -227,16 +248,33 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -253,7 +291,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E9"/>
+  <dimension ref="A2:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,6 +677,9 @@
       <c r="D3" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="E3" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -651,6 +694,9 @@
       <c r="D4" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="E4" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -665,7 +711,7 @@
       <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="10" t="s">
         <v>18</v>
       </c>
     </row>
@@ -721,7 +767,47 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="D9" s="1"/>
+      <c r="E9" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>9</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
-commit as of (3/4/2020) - code improvements - google api's
</commit_message>
<xml_diff>
--- a/doc/PusherDetails.xlsx
+++ b/doc/PusherDetails.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA1375C-3A86-44E7-954E-0D93740BEC09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>Sr No.</t>
   </si>
@@ -154,12 +153,6 @@
     <t>Add language</t>
   </si>
   <si>
-    <t>delete language</t>
-  </si>
-  <si>
-    <t>Update Organization setting</t>
-  </si>
-  <si>
     <t>ORG_SETTING_PUSHER</t>
   </si>
   <si>
@@ -167,13 +160,99 @@
   </si>
   <si>
     <t>NOTIFY_USER</t>
+  </si>
+  <si>
+    <t>Operation Name</t>
+  </si>
+  <si>
+    <t>DELETE_LANGUAGE_PUSHER</t>
+  </si>
+  <si>
+    <t>{
+  "op": "ADD_LANGUAGE_PUSHER",
+  "orgSettingDTO": {
+    "smsTemplateDTO": [
+      {
+        "templateText": "G_name #G_rank: There are P_ahead parties ahead of you w/ approx.",
+        "level": 1,
+        "languageID": 1,
+        "levelName": "Check-in"
+      },
+......
+    ],
+    "languageList": [
+      {
+        "langId": 1,
+        "langName": "English",
+        "langIsoCode": "en",
+        "languageMap": {
+          "enter_name_error": "Error! Please enter a valid name",
+      },
+      .......
+    ]}}</t>
+  </si>
+  <si>
+    <t>Delete Language</t>
+  </si>
+  <si>
+    <t>Organization Setting</t>
+  </si>
+  <si>
+    <t>{
+  "op": "ORG_SETTING_PUSHER",
+  "orgSettingDTO": {
+    "orgId": 82,
+    "seatingPreference": [
+      {
+        "prefValueId": 39,   "prefValue": "Patio",
+        "prefKey": "patio"
+      }  ], "marketingPreference": [
+      { "prefValueId": 45, "prefValue": "Facebook",
+        "prefKey": "facebook"
+      }
+    ], "notifyFirst": 0,   "smsTemplateDTO": [
+      {  "smsTemplateID": 0, "templateText": "hi",
+        "level": 1, "languageID": 1,
+        "levelName": "string"
+      }
+    ], "languageList": [
+      {
+        "langId": 1,  "langName": "English",
+        "langIsoCode": "en","languageMap": {}
+      } ],
+    "defaultLanguage": 1,   "pplBifurcation": "Y"
+  }}</t>
+  </si>
+  <si>
+    <t>{"op": "DELETE_LANGUAGE_PUSHER",
+  "orgSettingDTO": {
+    "smsTemplateDTO": [
+      {
+        "smsTemplateID": 1599,
+        "templateText": "G_name #G_rank: Il y a.",
+        "level": 1,
+        "languageID": 34,
+        "levelName": "Check-in"
+      },
+      .......
+    ],
+    "languageList": [
+      {
+        "langId": 34,
+        "langName": "French",
+        "langIsoCode": "fr",
+        "languageMap": {
+            "enter_name_error": "Error! Please enter a valid name",         
+      },
+   ........
+   ]}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,12 +267,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -210,7 +283,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -244,39 +317,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -292,8 +338,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,7 +404,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -386,27 +436,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -438,24 +470,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -631,183 +645,212 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
     <col min="2" max="2" width="32.7109375" customWidth="1"/>
     <col min="3" max="3" width="33.140625" customWidth="1"/>
-    <col min="4" max="4" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="48.28515625" customWidth="1"/>
     <col min="5" max="5" width="44.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="E3" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="165">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="60">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="315" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    <row r="6" spans="1:5" ht="315">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="285" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+    <row r="7" spans="1:5" ht="285">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="195" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+    <row r="8" spans="1:5" ht="195">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+    <row r="9" spans="1:5" ht="360">
+      <c r="A9" s="9">
         <v>7</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="11" t="s">
+      <c r="D9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+    <row r="10" spans="1:5" ht="345">
+      <c r="A10" s="9">
         <v>8</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="360">
+      <c r="A11" s="9">
+        <v>9</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
-        <v>9</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="12" t="s">
-        <v>26</v>
-      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="10"/>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -816,24 +859,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>